<commit_message>
Import formdata using custom_command
</commit_message>
<xml_diff>
--- a/managementCommandsFiles/FormsFeb12.xlsx
+++ b/managementCommandsFiles/FormsFeb12.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="257">
   <si>
     <t xml:space="preserve">Form ID</t>
   </si>
@@ -331,9 +331,15 @@
     <t xml:space="preserve">48</t>
   </si>
   <si>
+    <t xml:space="preserve">Lots1</t>
+  </si>
+  <si>
     <t xml:space="preserve">49</t>
   </si>
   <si>
+    <t xml:space="preserve">Serial Number1</t>
+  </si>
+  <si>
     <t xml:space="preserve">50</t>
   </si>
   <si>
@@ -343,6 +349,9 @@
     <t xml:space="preserve">51</t>
   </si>
   <si>
+    <t xml:space="preserve">Container Type1</t>
+  </si>
+  <si>
     <t xml:space="preserve">52</t>
   </si>
   <si>
@@ -376,6 +385,9 @@
     <t xml:space="preserve">57</t>
   </si>
   <si>
+    <t xml:space="preserve">Communication1</t>
+  </si>
+  <si>
     <t xml:space="preserve">58</t>
   </si>
   <si>
@@ -562,6 +574,9 @@
     <t xml:space="preserve">83</t>
   </si>
   <si>
+    <t xml:space="preserve">Lists1</t>
+  </si>
+  <si>
     <t xml:space="preserve">84</t>
   </si>
   <si>
@@ -625,6 +640,9 @@
     <t xml:space="preserve">93</t>
   </si>
   <si>
+    <t xml:space="preserve">Settings1</t>
+  </si>
+  <si>
     <t xml:space="preserve">94</t>
   </si>
   <si>
@@ -724,15 +742,21 @@
     <t xml:space="preserve">110</t>
   </si>
   <si>
+    <t xml:space="preserve">Blogs1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Blogs</t>
   </si>
   <si>
-    <t xml:space="preserve">111</t>
-  </si>
-  <si>
     <t xml:space="preserve">112</t>
   </si>
   <si>
+    <t xml:space="preserve">Tags1</t>
+  </si>
+  <si>
     <t xml:space="preserve">113</t>
   </si>
   <si>
@@ -748,6 +772,9 @@
     <t xml:space="preserve">115</t>
   </si>
   <si>
+    <t xml:space="preserve">Channels1</t>
+  </si>
+  <si>
     <t xml:space="preserve">116</t>
   </si>
   <si>
@@ -755,6 +782,9 @@
   </si>
   <si>
     <t xml:space="preserve">117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tags2</t>
   </si>
   <si>
     <t xml:space="preserve">118</t>
@@ -962,12 +992,12 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+      <selection pane="bottomLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.35546875" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
@@ -975,7 +1005,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="16.36"/>
   </cols>
   <sheetData>
@@ -1624,7 +1654,7 @@
         <v>102</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="3"/>
@@ -1634,10 +1664,10 @@
     </row>
     <row r="50" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="3"/>
@@ -1647,10 +1677,10 @@
     </row>
     <row r="51" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="3"/>
@@ -1660,10 +1690,10 @@
     </row>
     <row r="52" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="3"/>
@@ -1673,10 +1703,10 @@
     </row>
     <row r="53" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="3"/>
@@ -1686,10 +1716,10 @@
     </row>
     <row r="54" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="3"/>
@@ -1699,10 +1729,10 @@
     </row>
     <row r="55" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="3"/>
@@ -1712,10 +1742,10 @@
     </row>
     <row r="56" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="3"/>
@@ -1725,10 +1755,10 @@
     </row>
     <row r="57" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="3"/>
@@ -1738,10 +1768,10 @@
     </row>
     <row r="58" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
@@ -1751,10 +1781,10 @@
     </row>
     <row r="59" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
@@ -1764,10 +1794,10 @@
     </row>
     <row r="60" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
@@ -1777,10 +1807,10 @@
     </row>
     <row r="61" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
@@ -1790,10 +1820,10 @@
     </row>
     <row r="62" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
@@ -1803,10 +1833,10 @@
     </row>
     <row r="63" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
@@ -1816,10 +1846,10 @@
     </row>
     <row r="64" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
@@ -1829,10 +1859,10 @@
     </row>
     <row r="65" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
@@ -1842,10 +1872,10 @@
     </row>
     <row r="66" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
@@ -1855,10 +1885,10 @@
     </row>
     <row r="67" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
@@ -1868,10 +1898,10 @@
     </row>
     <row r="68" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
@@ -1881,10 +1911,10 @@
     </row>
     <row r="69" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
@@ -1894,10 +1924,10 @@
     </row>
     <row r="70" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
@@ -1907,125 +1937,125 @@
     </row>
     <row r="71" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
     </row>
     <row r="72" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="6" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
     </row>
     <row r="74" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="6" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
@@ -2035,10 +2065,10 @@
     </row>
     <row r="79" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
@@ -2048,10 +2078,10 @@
     </row>
     <row r="80" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
@@ -2061,10 +2091,10 @@
     </row>
     <row r="81" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
@@ -2074,10 +2104,10 @@
     </row>
     <row r="82" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
@@ -2087,10 +2117,10 @@
     </row>
     <row r="83" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
@@ -2100,10 +2130,10 @@
     </row>
     <row r="84" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
@@ -2113,10 +2143,10 @@
     </row>
     <row r="85" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
@@ -2126,10 +2156,10 @@
     </row>
     <row r="86" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
@@ -2139,10 +2169,10 @@
     </row>
     <row r="87" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
@@ -2152,10 +2182,10 @@
     </row>
     <row r="88" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
@@ -2165,10 +2195,10 @@
     </row>
     <row r="89" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
@@ -2178,10 +2208,10 @@
     </row>
     <row r="90" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
@@ -2191,10 +2221,10 @@
     </row>
     <row r="91" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
@@ -2204,27 +2234,27 @@
     </row>
     <row r="92" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="17" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F92" s="16"/>
       <c r="G92" s="5"/>
     </row>
     <row r="93" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
@@ -2234,10 +2264,10 @@
     </row>
     <row r="94" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>141</v>
+        <v>206</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
@@ -2247,10 +2277,10 @@
     </row>
     <row r="95" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
@@ -2260,10 +2290,10 @@
     </row>
     <row r="96" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
@@ -2273,10 +2303,10 @@
     </row>
     <row r="97" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
@@ -2286,10 +2316,10 @@
     </row>
     <row r="98" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
@@ -2299,10 +2329,10 @@
     </row>
     <row r="99" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
@@ -2312,10 +2342,10 @@
     </row>
     <row r="100" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
@@ -2325,10 +2355,10 @@
     </row>
     <row r="101" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C101" s="4"/>
       <c r="D101" s="5"/>
@@ -2338,10 +2368,10 @@
     </row>
     <row r="102" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C102" s="4"/>
       <c r="D102" s="5"/>
@@ -2351,10 +2381,10 @@
     </row>
     <row r="103" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C103" s="4"/>
       <c r="D103" s="5"/>
@@ -2364,10 +2394,10 @@
     </row>
     <row r="104" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="5"/>
@@ -2377,10 +2407,10 @@
     </row>
     <row r="105" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C105" s="4"/>
       <c r="D105" s="5"/>
@@ -2390,10 +2420,10 @@
     </row>
     <row r="106" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C106" s="4"/>
       <c r="D106" s="5"/>
@@ -2403,10 +2433,10 @@
     </row>
     <row r="107" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="5"/>
@@ -2416,10 +2446,10 @@
     </row>
     <row r="108" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="5"/>
@@ -2429,10 +2459,10 @@
     </row>
     <row r="109" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="5"/>
@@ -2442,10 +2472,10 @@
     </row>
     <row r="110" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="5"/>
@@ -2455,10 +2485,10 @@
     </row>
     <row r="111" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="5"/>
@@ -2468,10 +2498,10 @@
     </row>
     <row r="112" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="5"/>
@@ -2481,10 +2511,10 @@
     </row>
     <row r="113" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="5"/>
@@ -2494,10 +2524,10 @@
     </row>
     <row r="114" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="5"/>
@@ -2507,10 +2537,10 @@
     </row>
     <row r="115" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C115" s="4"/>
       <c r="D115" s="5"/>
@@ -2520,10 +2550,10 @@
     </row>
     <row r="116" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>123</v>
+        <v>250</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="5"/>
@@ -2533,10 +2563,10 @@
     </row>
     <row r="117" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="5"/>
@@ -2546,10 +2576,10 @@
     </row>
     <row r="118" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>195</v>
+        <v>254</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="5"/>
@@ -2559,10 +2589,10 @@
     </row>
     <row r="119" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="5"/>

</xml_diff>